<commit_message>
got some simulation results
</commit_message>
<xml_diff>
--- a/simulation results/week4/capacitor values with and without interleaving.xlsx
+++ b/simulation results/week4/capacitor values with and without interleaving.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t xml:space="preserve">Voltage swing </t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>8888VA  0.9pf lagging per inverter</t>
-  </si>
-  <si>
-    <t>3 level SPWM (ma = 1, mf = 41)</t>
   </si>
   <si>
     <r>
@@ -70,12 +67,113 @@
   <si>
     <t>300µF (2 pieces for 2 inverters)</t>
   </si>
+  <si>
+    <t>3 level SPWM (ma = 1, mf = 41,fundf = 50hz)</t>
+  </si>
+  <si>
+    <t>269.5 - 268.1 (Vpp = 1.47V)</t>
+  </si>
+  <si>
+    <t>268.4 - 267.8 (Vpp = 0.6V)</t>
+  </si>
+  <si>
+    <t>250µF (2 pieces for 2 inverters)</t>
+  </si>
+  <si>
+    <t>1400µF (4 pieces for 2 inverters)</t>
+  </si>
+  <si>
+    <t>269.6 - 269.4 (Vpp = 0.22 V)</t>
+  </si>
+  <si>
+    <t>100µF  (4 pieces for 2 inverters)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">268.8 - 268.5 (Vpp = 0.3 V)                  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t xml:space="preserve">      269.4 - 269.2 (Vpp = 0.15 V) with same total load</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">280µF (2 pieces for 2 inverters)                 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t xml:space="preserve">      80µF (2 pieces for 2 inverters) with same total load</t>
+    </r>
+  </si>
+  <si>
+    <t>2 level SPWM (ma = 1, mf = 41,fundf = 50hz)</t>
+  </si>
+  <si>
+    <t>269.4 - 268.8 (Vpp = 0.63V)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">268.5 - 267.7 (Vpp = 0.74V)                    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t xml:space="preserve">    269.2 - 268.9 (Vpp = 0.37 V) with same total load</t>
+    </r>
+  </si>
+  <si>
+    <t>270µF (4 pieces for 2 inverters)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">430µF (2 pieces for 2 inverters)                     </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  60µF (2 pieces for 2 inverters) with same total load</t>
+    </r>
+  </si>
+  <si>
+    <t>3 level SVPWM (ma = 1, swf = 2050hz,fundf = 50hz)</t>
+  </si>
+  <si>
+    <t>2 level SVPWM (ma = 1, swf = 2050hz,fundf = 50hz)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +197,23 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -120,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -142,6 +257,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,67 +578,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2716843C-4BF8-4DB4-AA36-F330CE592E11}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="35.42578125" style="3" customWidth="1"/>
-    <col min="3" max="5" width="35.42578125" customWidth="1"/>
+    <col min="1" max="2" width="42.42578125" style="3" customWidth="1"/>
+    <col min="3" max="4" width="42.42578125" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
     <col min="6" max="8" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+    <row r="1" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
       <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
+      <c r="E2"/>
     </row>
     <row r="3" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
@@ -525,69 +648,175 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+    <row r="6" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+    <row r="10" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+    <row r="11" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+    <row r="12" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+    <row r="13" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+    <row r="14" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+    <row r="15" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
     </row>
+    <row r="16" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A6:D6"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>